<commit_message>
Præver at slippe arket
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_PRO_B\VejlederMatrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_Pro_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F6505F2-A56D-40C7-9584-941B1015BAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5474E837-5B1F-4C21-BEB9-1203FACAAB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Vejleder1</t>
+  </si>
+  <si>
+    <t>Vejleder2</t>
+  </si>
+  <si>
+    <t>Møder</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,45 +396,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3351F8D1-261B-4E86-BDD0-503D41E31D76}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="F3:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="H3" t="s">
         <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quite far now, has all the information it needs for the processing
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_PRO_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCF9D4E-606B-405C-A0BE-7F9DC202071D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B9E8B-1E63-4510-9A17-F543B6210928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="7200" yWindow="600" windowWidth="21600" windowHeight="11295" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Så mangler kun outputtet
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_PRO_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B9E8B-1E63-4510-9A17-F543B6210928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3722E36C-2872-4817-974B-E62C1E86B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="600" windowWidth="21600" windowHeight="11295" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="0" yWindow="1875" windowWidth="8700" windowHeight="11385" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId1"/>
+    <sheet name="Ark1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>Vejleder1</t>
   </si>
@@ -60,6 +61,12 @@
   </si>
   <si>
     <t>SOD</t>
+  </si>
+  <si>
+    <t>Vejleder 1:</t>
+  </si>
+  <si>
+    <t>Vejleder 2:</t>
   </si>
 </sst>
 </file>
@@ -410,10 +417,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF8305F-3A3B-40E9-BFAE-78E2FE68DC6B}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3351F8D1-261B-4E86-BDD0-503D41E31D76}">
   <dimension ref="C3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tror fandme den virker nu!
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_PRO_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0CF2E9-014B-4188-9047-D055CD9A2F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA046774-4071-4A75-8106-600AED56D76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="600" windowWidth="21600" windowHeight="11295" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultat" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="11">
   <si>
     <t>Vejleder1</t>
   </si>
@@ -69,25 +69,7 @@
     <t>Vejleder 2:</t>
   </si>
   <si>
-    <t>Optaget (MKR og DRK)</t>
-  </si>
-  <si>
-    <t>Optaget (DRK og LOD)</t>
-  </si>
-  <si>
-    <t>Optaget (UOP og MKR)</t>
-  </si>
-  <si>
-    <t>Optaget (LOD og SOD)</t>
-  </si>
-  <si>
-    <t>Optaget (SOD og UOP)</t>
-  </si>
-  <si>
-    <t>Optaget (SOD og MKR)</t>
-  </si>
-  <si>
-    <t>Optaget (DRK og MKR)</t>
+    <t>Optaget</t>
   </si>
 </sst>
 </file>
@@ -439,13 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF68456-7D0C-4F5A-8AEB-D7304885B530}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -453,18 +442,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -472,32 +464,65 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -505,40 +530,73 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
+      <c r="M9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Emil kom med gode forslag
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_PRO_B\VejlederMatrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_Pro_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA046774-4071-4A75-8106-600AED56D76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FDC9F1-7CED-495C-AD04-AD1E194E051F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="0" yWindow="1875" windowWidth="8700" windowHeight="11385" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultat" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Så Duer Den Fandme (feat. Marcell)
</commit_message>
<xml_diff>
--- a/VejlederMatrix.xlsx
+++ b/VejlederMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC_Pro_B\VejlederMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FDC9F1-7CED-495C-AD04-AD1E194E051F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86C32F4-F588-44C0-A5CD-08C5E04B6952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1875" windowWidth="8700" windowHeight="11385" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
+    <workbookView xWindow="345" yWindow="2220" windowWidth="8700" windowHeight="11385" activeTab="1" xr2:uid="{FB9A82ED-5DA7-47B6-ADC6-6C7B5F56D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultat" sheetId="2" r:id="rId1"/>
@@ -37,32 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="11">
-  <si>
-    <t>Vejleder1</t>
-  </si>
-  <si>
-    <t>Vejleder2</t>
-  </si>
-  <si>
-    <t>Møder</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="21">
   <si>
     <t>MKR</t>
   </si>
   <si>
-    <t>DRK</t>
-  </si>
-  <si>
-    <t>UOP</t>
-  </si>
-  <si>
-    <t>LOD</t>
-  </si>
-  <si>
-    <t>SOD</t>
-  </si>
-  <si>
     <t>Vejleder 1:</t>
   </si>
   <si>
@@ -70,6 +49,57 @@
   </si>
   <si>
     <t>Optaget</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>THFI</t>
+  </si>
+  <si>
+    <t>BSE</t>
+  </si>
+  <si>
+    <t>DWX</t>
+  </si>
+  <si>
+    <t>KU</t>
+  </si>
+  <si>
+    <t>ILR</t>
+  </si>
+  <si>
+    <t>BEJE</t>
+  </si>
+  <si>
+    <t>NHJ</t>
+  </si>
+  <si>
+    <t>MKJA</t>
+  </si>
+  <si>
+    <t>JEMA</t>
+  </si>
+  <si>
+    <t>JJJ</t>
+  </si>
+  <si>
+    <t>KRA</t>
+  </si>
+  <si>
+    <t>KIAN</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>LBI</t>
+  </si>
+  <si>
+    <t>CU</t>
   </si>
 </sst>
 </file>
@@ -421,9 +451,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF68456-7D0C-4F5A-8AEB-D7304885B530}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
@@ -436,64 +466,85 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -501,102 +552,415 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
         <v>3</v>
       </c>
       <c r="S7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
       </c>
       <c r="N8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="M9" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T9" t="s">
-        <v>10</v>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -606,10 +970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3351F8D1-261B-4E86-BDD0-503D41E31D76}">
-  <dimension ref="C3:E11"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,102 +982,322 @@
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
         <v>3</v>
       </c>
     </row>

</xml_diff>